<commit_message>
Edits to heritability clustering script.
</commit_message>
<xml_diff>
--- a/Plant_Materials/S2MET_project_entries.xlsx
+++ b/Plant_Materials/S2MET_project_entries.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="465">
   <si>
     <t>06AB-08</t>
   </si>
@@ -1419,6 +1419,9 @@
   </si>
   <si>
     <t>07WA-614.12</t>
+  </si>
+  <si>
+    <t>M2</t>
   </si>
 </sst>
 </file>
@@ -1787,18 +1790,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="K198" sqref="K198"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E186" sqref="E186:E234"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>232</v>
       </c>
@@ -1818,7 +1821,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1858,7 +1861,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1878,7 +1881,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1898,7 +1901,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1918,7 +1921,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1938,7 +1941,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1958,7 +1961,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1978,7 +1981,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1998,7 +2001,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2018,7 +2021,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2038,7 +2041,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2058,7 +2061,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2078,7 +2081,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2098,7 +2101,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2118,7 +2121,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2138,7 +2141,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2158,7 +2161,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2178,7 +2181,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2198,7 +2201,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2218,7 +2221,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2238,7 +2241,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2258,7 +2261,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2278,7 +2281,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -2298,7 +2301,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2318,7 +2321,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2338,7 +2341,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2358,7 +2361,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2378,7 +2381,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2398,7 +2401,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2418,7 +2421,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2438,7 +2441,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2458,7 +2461,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2478,7 +2481,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -2498,7 +2501,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2518,7 +2521,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -2538,7 +2541,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2558,7 +2561,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -2578,7 +2581,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -2598,7 +2601,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -2618,7 +2621,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -2638,7 +2641,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -2658,7 +2661,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2678,7 +2681,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -2698,7 +2701,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -2718,7 +2721,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -2738,7 +2741,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -2758,7 +2761,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -2778,7 +2781,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2798,7 +2801,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2818,7 +2821,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2838,7 +2841,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -2858,7 +2861,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -2878,7 +2881,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -2898,7 +2901,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -2918,7 +2921,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2938,7 +2941,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -2958,7 +2961,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -2978,7 +2981,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -2998,7 +3001,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -3018,7 +3021,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -3038,7 +3041,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -3058,7 +3061,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -3078,7 +3081,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -3098,7 +3101,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -3118,7 +3121,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -3138,7 +3141,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -3158,7 +3161,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -3178,7 +3181,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -3198,7 +3201,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -3218,7 +3221,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -3238,7 +3241,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -3258,7 +3261,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -3278,7 +3281,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -3298,7 +3301,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -3318,7 +3321,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -3338,7 +3341,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -3358,7 +3361,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -3378,7 +3381,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -3398,7 +3401,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -3418,7 +3421,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -3438,7 +3441,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -3458,7 +3461,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -3478,7 +3481,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -3498,7 +3501,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -3518,7 +3521,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -3538,7 +3541,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>86</v>
       </c>
@@ -3558,7 +3561,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -3578,7 +3581,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -3598,7 +3601,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -3618,7 +3621,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -3638,7 +3641,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -3658,7 +3661,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -3678,7 +3681,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -3698,7 +3701,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -3718,7 +3721,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -3738,7 +3741,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -3758,7 +3761,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -3778,7 +3781,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -3798,7 +3801,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -3818,7 +3821,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>100</v>
       </c>
@@ -3838,7 +3841,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -3858,7 +3861,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -3878,7 +3881,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>103</v>
       </c>
@@ -3898,7 +3901,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>104</v>
       </c>
@@ -3918,7 +3921,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>105</v>
       </c>
@@ -3938,7 +3941,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>106</v>
       </c>
@@ -3958,7 +3961,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -3978,7 +3981,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>108</v>
       </c>
@@ -3998,7 +4001,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>109</v>
       </c>
@@ -4018,7 +4021,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -4038,7 +4041,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>111</v>
       </c>
@@ -4058,7 +4061,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>112</v>
       </c>
@@ -4078,7 +4081,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>113</v>
       </c>
@@ -4098,7 +4101,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>114</v>
       </c>
@@ -4118,7 +4121,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>115</v>
       </c>
@@ -4138,7 +4141,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>116</v>
       </c>
@@ -4158,7 +4161,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>117</v>
       </c>
@@ -4178,7 +4181,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>118</v>
       </c>
@@ -4198,7 +4201,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>119</v>
       </c>
@@ -4218,7 +4221,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>120</v>
       </c>
@@ -4238,7 +4241,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>121</v>
       </c>
@@ -4258,7 +4261,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>122</v>
       </c>
@@ -4278,7 +4281,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>123</v>
       </c>
@@ -4298,7 +4301,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>124</v>
       </c>
@@ -4318,7 +4321,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -4338,7 +4341,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>126</v>
       </c>
@@ -4358,7 +4361,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>127</v>
       </c>
@@ -4378,7 +4381,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>128</v>
       </c>
@@ -4398,7 +4401,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>129</v>
       </c>
@@ -4418,7 +4421,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>130</v>
       </c>
@@ -4438,7 +4441,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>131</v>
       </c>
@@ -4458,7 +4461,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>132</v>
       </c>
@@ -4478,7 +4481,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>133</v>
       </c>
@@ -4498,7 +4501,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>134</v>
       </c>
@@ -4518,7 +4521,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>135</v>
       </c>
@@ -4538,7 +4541,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>136</v>
       </c>
@@ -4558,7 +4561,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>137</v>
       </c>
@@ -4578,7 +4581,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>138</v>
       </c>
@@ -4598,7 +4601,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>139</v>
       </c>
@@ -4618,7 +4621,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>140</v>
       </c>
@@ -4638,7 +4641,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>141</v>
       </c>
@@ -4658,7 +4661,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>142</v>
       </c>
@@ -4678,7 +4681,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>143</v>
       </c>
@@ -4698,7 +4701,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>144</v>
       </c>
@@ -4718,7 +4721,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>145</v>
       </c>
@@ -4738,7 +4741,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>146</v>
       </c>
@@ -4758,7 +4761,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>147</v>
       </c>
@@ -4778,7 +4781,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>148</v>
       </c>
@@ -4798,7 +4801,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>149</v>
       </c>
@@ -4818,7 +4821,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>150</v>
       </c>
@@ -4838,7 +4841,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>151</v>
       </c>
@@ -4858,7 +4861,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>152</v>
       </c>
@@ -4878,7 +4881,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>153</v>
       </c>
@@ -4898,7 +4901,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>154</v>
       </c>
@@ -4918,7 +4921,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>155</v>
       </c>
@@ -4938,7 +4941,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>156</v>
       </c>
@@ -4958,7 +4961,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>157</v>
       </c>
@@ -4978,7 +4981,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>158</v>
       </c>
@@ -4998,7 +5001,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>159</v>
       </c>
@@ -5018,7 +5021,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
         <v>160</v>
       </c>
@@ -5038,7 +5041,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>161</v>
       </c>
@@ -5058,7 +5061,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>162</v>
       </c>
@@ -5078,7 +5081,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>163</v>
       </c>
@@ -5098,7 +5101,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
         <v>164</v>
       </c>
@@ -5118,7 +5121,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>165</v>
       </c>
@@ -5138,7 +5141,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
         <v>166</v>
       </c>
@@ -5158,7 +5161,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>167</v>
       </c>
@@ -5178,7 +5181,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
         <v>168</v>
       </c>
@@ -5198,7 +5201,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>169</v>
       </c>
@@ -5218,7 +5221,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
         <v>170</v>
       </c>
@@ -5238,7 +5241,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>171</v>
       </c>
@@ -5258,7 +5261,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
         <v>172</v>
       </c>
@@ -5278,7 +5281,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>173</v>
       </c>
@@ -5298,7 +5301,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
         <v>174</v>
       </c>
@@ -5318,7 +5321,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
         <v>175</v>
       </c>
@@ -5338,7 +5341,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
         <v>176</v>
       </c>
@@ -5358,7 +5361,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
         <v>177</v>
       </c>
@@ -5378,7 +5381,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
         <v>178</v>
       </c>
@@ -5398,7 +5401,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
         <v>179</v>
       </c>
@@ -5418,7 +5421,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
         <v>180</v>
       </c>
@@ -5438,7 +5441,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
         <v>181</v>
       </c>
@@ -5458,7 +5461,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
         <v>182</v>
       </c>
@@ -5478,7 +5481,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
         <v>231</v>
       </c>
@@ -5492,13 +5495,13 @@
         <v>269</v>
       </c>
       <c r="E185" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F185" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
         <v>230</v>
       </c>
@@ -5512,13 +5515,13 @@
         <v>269</v>
       </c>
       <c r="E186" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F186" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
         <v>229</v>
       </c>
@@ -5532,13 +5535,13 @@
         <v>269</v>
       </c>
       <c r="E187" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F187" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
         <v>228</v>
       </c>
@@ -5552,13 +5555,13 @@
         <v>269</v>
       </c>
       <c r="E188" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F188" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
         <v>227</v>
       </c>
@@ -5572,13 +5575,13 @@
         <v>269</v>
       </c>
       <c r="E189" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F189" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
         <v>226</v>
       </c>
@@ -5592,13 +5595,13 @@
         <v>269</v>
       </c>
       <c r="E190" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F190" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
         <v>225</v>
       </c>
@@ -5612,13 +5615,13 @@
         <v>269</v>
       </c>
       <c r="E191" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F191" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
         <v>224</v>
       </c>
@@ -5632,13 +5635,13 @@
         <v>269</v>
       </c>
       <c r="E192" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F192" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>223</v>
       </c>
@@ -5652,13 +5655,13 @@
         <v>269</v>
       </c>
       <c r="E193" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F193" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>222</v>
       </c>
@@ -5672,13 +5675,13 @@
         <v>269</v>
       </c>
       <c r="E194" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F194" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>221</v>
       </c>
@@ -5692,13 +5695,13 @@
         <v>269</v>
       </c>
       <c r="E195" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F195" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>220</v>
       </c>
@@ -5712,13 +5715,13 @@
         <v>269</v>
       </c>
       <c r="E196" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F196" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>264</v>
       </c>
@@ -5732,13 +5735,13 @@
         <v>269</v>
       </c>
       <c r="E197" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F197" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>219</v>
       </c>
@@ -5752,13 +5755,13 @@
         <v>269</v>
       </c>
       <c r="E198" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F198" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>218</v>
       </c>
@@ -5772,13 +5775,13 @@
         <v>269</v>
       </c>
       <c r="E199" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F199" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>217</v>
       </c>
@@ -5792,13 +5795,13 @@
         <v>269</v>
       </c>
       <c r="E200" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F200" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>216</v>
       </c>
@@ -5812,13 +5815,13 @@
         <v>269</v>
       </c>
       <c r="E201" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F201" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
         <v>215</v>
       </c>
@@ -5832,13 +5835,13 @@
         <v>269</v>
       </c>
       <c r="E202" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F202" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>214</v>
       </c>
@@ -5852,13 +5855,13 @@
         <v>269</v>
       </c>
       <c r="E203" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F203" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
         <v>213</v>
       </c>
@@ -5872,13 +5875,13 @@
         <v>269</v>
       </c>
       <c r="E204" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F204" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>212</v>
       </c>
@@ -5892,13 +5895,13 @@
         <v>269</v>
       </c>
       <c r="E205" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F205" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
         <v>211</v>
       </c>
@@ -5912,13 +5915,13 @@
         <v>269</v>
       </c>
       <c r="E206" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F206" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
         <v>210</v>
       </c>
@@ -5932,13 +5935,13 @@
         <v>269</v>
       </c>
       <c r="E207" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F207" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
         <v>209</v>
       </c>
@@ -5952,13 +5955,13 @@
         <v>269</v>
       </c>
       <c r="E208" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F208" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
         <v>208</v>
       </c>
@@ -5972,13 +5975,13 @@
         <v>269</v>
       </c>
       <c r="E209" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F209" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A210" t="s">
         <v>207</v>
       </c>
@@ -5992,13 +5995,13 @@
         <v>269</v>
       </c>
       <c r="E210" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F210" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
         <v>206</v>
       </c>
@@ -6012,13 +6015,13 @@
         <v>269</v>
       </c>
       <c r="E211" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F211" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
         <v>205</v>
       </c>
@@ -6032,13 +6035,13 @@
         <v>269</v>
       </c>
       <c r="E212" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F212" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
         <v>204</v>
       </c>
@@ -6052,13 +6055,13 @@
         <v>269</v>
       </c>
       <c r="E213" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F213" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A214" t="s">
         <v>203</v>
       </c>
@@ -6072,13 +6075,13 @@
         <v>269</v>
       </c>
       <c r="E214" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F214" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A215" t="s">
         <v>202</v>
       </c>
@@ -6092,13 +6095,13 @@
         <v>269</v>
       </c>
       <c r="E215" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F215" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A216" t="s">
         <v>201</v>
       </c>
@@ -6112,13 +6115,13 @@
         <v>269</v>
       </c>
       <c r="E216" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F216" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
         <v>200</v>
       </c>
@@ -6132,13 +6135,13 @@
         <v>269</v>
       </c>
       <c r="E217" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F217" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
         <v>199</v>
       </c>
@@ -6152,13 +6155,13 @@
         <v>269</v>
       </c>
       <c r="E218" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F218" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
         <v>198</v>
       </c>
@@ -6172,13 +6175,13 @@
         <v>269</v>
       </c>
       <c r="E219" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F219" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A220" t="s">
         <v>197</v>
       </c>
@@ -6192,13 +6195,13 @@
         <v>269</v>
       </c>
       <c r="E220" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F220" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
         <v>196</v>
       </c>
@@ -6212,13 +6215,13 @@
         <v>269</v>
       </c>
       <c r="E221" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F221" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
         <v>195</v>
       </c>
@@ -6232,13 +6235,13 @@
         <v>269</v>
       </c>
       <c r="E222" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F222" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A223" t="s">
         <v>194</v>
       </c>
@@ -6252,13 +6255,13 @@
         <v>269</v>
       </c>
       <c r="E223" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F223" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
         <v>193</v>
       </c>
@@ -6272,13 +6275,13 @@
         <v>269</v>
       </c>
       <c r="E224" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F224" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
         <v>192</v>
       </c>
@@ -6292,13 +6295,13 @@
         <v>269</v>
       </c>
       <c r="E225" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F225" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
         <v>191</v>
       </c>
@@ -6312,13 +6315,13 @@
         <v>269</v>
       </c>
       <c r="E226" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F226" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A227" t="s">
         <v>190</v>
       </c>
@@ -6332,13 +6335,13 @@
         <v>269</v>
       </c>
       <c r="E227" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F227" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
         <v>189</v>
       </c>
@@ -6352,13 +6355,13 @@
         <v>269</v>
       </c>
       <c r="E228" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F228" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
         <v>188</v>
       </c>
@@ -6372,13 +6375,13 @@
         <v>269</v>
       </c>
       <c r="E229" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F229" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A230" t="s">
         <v>187</v>
       </c>
@@ -6392,13 +6395,13 @@
         <v>269</v>
       </c>
       <c r="E230" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F230" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A231" t="s">
         <v>186</v>
       </c>
@@ -6412,13 +6415,13 @@
         <v>269</v>
       </c>
       <c r="E231" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F231" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A232" t="s">
         <v>185</v>
       </c>
@@ -6432,13 +6435,13 @@
         <v>269</v>
       </c>
       <c r="E232" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F232" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A233" t="s">
         <v>184</v>
       </c>
@@ -6452,13 +6455,13 @@
         <v>269</v>
       </c>
       <c r="E233" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F233" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A234" t="s">
         <v>183</v>
       </c>
@@ -6472,13 +6475,13 @@
         <v>269</v>
       </c>
       <c r="E234" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="F234" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A235" t="s">
         <v>256</v>
       </c>
@@ -6495,7 +6498,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A236" t="s">
         <v>257</v>
       </c>
@@ -6512,7 +6515,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A237" t="s">
         <v>258</v>
       </c>
@@ -6529,7 +6532,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A238" t="s">
         <v>255</v>
       </c>
@@ -6546,7 +6549,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A239" t="s">
         <v>262</v>
       </c>
@@ -6563,7 +6566,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A240" t="s">
         <v>260</v>
       </c>
@@ -6580,7 +6583,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A241" t="s">
         <v>261</v>
       </c>
@@ -6597,7 +6600,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A242" t="s">
         <v>259</v>
       </c>
@@ -6614,7 +6617,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A243" t="s">
         <v>254</v>
       </c>
@@ -6631,7 +6634,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A244" t="s">
         <v>263</v>
       </c>
@@ -6648,7 +6651,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
         <v>270</v>
       </c>

</xml_diff>